<commit_message>
Updated the utterances file. On robot class added the posture gratitude and use this posture when the player is congruent on his choice and the robot is against its personality.
</commit_message>
<xml_diff>
--- a/SOP/Utterances/phrasesFavorPositive.xlsx
+++ b/SOP/Utterances/phrasesFavorPositive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie\Desktop\Git\Storytelling_SR\SOP\Utterances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68C92D0-033A-4E43-86F0-9AD51DE2ACB7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D5922C-14DF-477D-AFCD-5AEDD7E5FC56}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24015" xr2:uid="{E4B8DB12-B672-4611-9817-EB9A51AE5FB6}"/>
   </bookViews>
@@ -66,12 +66,6 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>PT:FAVOUR</t>
-  </si>
-  <si>
-    <t>EN:FAVOUR</t>
-  </si>
-  <si>
     <t>REPETITIONS</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Brilhante. Não espero outra decisão.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Pessoalmente, esta é a minha decisão favorita.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Esta decisão está completamente correta.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Horrível. A outra decisão é melhor.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Pessoalmente, prefiro a outra decisão.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Esta decisão está completamente incorreta.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
@@ -222,21 +210,12 @@
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  I understand your point of view and agree with it.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Definitely, this will help people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  I completely agree with you.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Wonderful. With this decision, you will save the people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Brilliant. I did not expect another decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Personally, this is my favourite decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  This decision is correct.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
@@ -267,18 +246,9 @@
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  This decision will not help people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Definitely, I disagree with you.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Wrong. With this decision, people will suffer.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Terrible. The other decision is better.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Personally, I prefer other decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  This decision is incorrect.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
@@ -304,6 +274,36 @@
   </si>
   <si>
     <t>EN:POSITIVE</t>
+  </si>
+  <si>
+    <t>PT:AGAINST</t>
+  </si>
+  <si>
+    <t>EN:AGAINST</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Pessoalmente; esta é a minha decisão favorita.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Pessoalmente; prefiro a outra decisão.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Definitely; this will help people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Wonderful. With this decision; you will save the people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Personally; this is myfavourite decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Definitely; I disagree with you.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Wrong. With this decision; people will suffer.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Personally; I prefer other decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
 </sst>
 </file>
@@ -847,14 +847,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC699C3-7B7D-494D-9389-830F8CDC6B9F}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="D55" sqref="D2:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="235.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -867,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -880,13 +880,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -894,13 +894,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -908,13 +908,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,13 +922,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -936,13 +936,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -950,13 +950,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -964,13 +964,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -978,13 +978,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -992,13 +992,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1006,13 +1006,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1020,13 +1020,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1034,13 +1034,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1048,13 +1048,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1062,13 +1062,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1076,13 +1076,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,13 +1090,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,13 +1104,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,13 +1118,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,13 +1132,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,13 +1146,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,13 +1160,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,13 +1174,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,13 +1188,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,13 +1202,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,13 +1216,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,13 +1230,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,13 +1244,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,13 +1258,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,13 +1272,13 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,13 +1286,13 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,13 +1300,13 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,13 +1314,13 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,13 +1328,13 @@
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,13 +1342,13 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,13 +1356,13 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,13 +1370,13 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,13 +1384,13 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,13 +1398,13 @@
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,13 +1412,13 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,13 +1426,13 @@
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,13 +1440,13 @@
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,13 +1454,13 @@
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1468,13 +1468,13 @@
         <v>45</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,13 +1482,13 @@
         <v>46</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1496,13 +1496,13 @@
         <v>47</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,13 +1510,13 @@
         <v>48</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1524,13 +1524,13 @@
         <v>49</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,13 +1538,13 @@
         <v>50</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,13 +1552,13 @@
         <v>51</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1566,13 +1566,13 @@
         <v>52</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1580,13 +1580,13 @@
         <v>53</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1594,13 +1594,13 @@
         <v>54</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1608,13 +1608,13 @@
         <v>55</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1622,13 +1622,13 @@
         <v>56</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
         <v>82</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1636,13 +1636,13 @@
         <v>57</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1650,13 +1650,13 @@
         <v>58</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1664,13 +1664,13 @@
         <v>59</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D58" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1678,13 +1678,13 @@
         <v>60</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1692,13 +1692,13 @@
         <v>61</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1706,13 +1706,13 @@
         <v>62</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,13 +1720,13 @@
         <v>63</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D62" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,13 +1734,13 @@
         <v>64</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1748,13 +1748,13 @@
         <v>65</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1762,13 +1762,13 @@
         <v>66</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D65" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1797,7 +1797,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,79 +1808,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>